<commit_message>
Get daily reddit data: Tue Nov 21 08:08:33 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_26.xlsx
+++ b/data/2023_11_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C427"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2148 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>180bv8b</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>I get my nails done, every few weeks. But I'd like suggestions for moisturizing</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180bv8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>180blxw</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>i am OBSESSED w this color changing polish!! fresh fill looking fresh 🤩 swipe to see the magic ✨🩷♥️</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180blxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>180be4v</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>What is the name of this tool?</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjkmzdfnkn1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>180aerq</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>How do care for my nails in winter?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180aerq/how_do_care_for_my_nails_in_winter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1809gu2</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Question!</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w665172tym1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>18093hz</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>#1, #2, or #3? 🎄❄️☃️ ps. I did these all myself!</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cstrt9zyum1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>18090ai</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Hey friends, please help a girl out here 😛 Square or oval for me? Thanks in advance.</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18090ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1808arm</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>First time getting gems !</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1808arm</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>18086s4</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Can I use this under full cover soft gel tips? Do I need anything else?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16mjcu0plm1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1808110</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Slightly better photos!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1808110</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1806s1m</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>DIY Acrylics!</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nx6km8vl8m1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1806fvz</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>This green is one of my favorites now! I did my own polygel set 😊</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1806fvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1805y32</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>My first polygel nails</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vizxmr721m1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1805sgd</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Is it normal to file under the nail until it’s gone?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bzesy0nzl1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1805deb</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Base coat + 2 layers top coat: why does top coat create this stripy texture? Looks awful :( Is it because I mistakenly shook the bottle beforehand? There are bubbles all on/around the brush in the bottle...</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k1ci0voxvl1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1805899</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>floral set i did on myself</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1805899</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1805758</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>First time doing my own nails😅</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8s72pieul1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1804zr3</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Jelly rainbow nails 🌈</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1804zr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1803w2k</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Tips for first time gel nails @ home</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1803w2k/tips_for_first_time_gel_nails_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>18039et</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Getting into my coquette era</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18039et</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>180345w</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Did these myself!! So proud</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180345w</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1802k74</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>my first blinged out set!</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g4ecmxsa8l1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1802bkg</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>This video has no filter…</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/16q1canc6l1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>180256b</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>17m. Stole my moms red nail polish 😂</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180256b</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1801nam</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Update! Went with red ☺️</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zjux5hc1l1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1801lg1</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Maple leaf 🍁</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9iw2516z0l1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1801i73</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Third set on myself!</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkx90fdb0l1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>180125i</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Gel or semi-permanent polish for first time manicure?</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180125i/gel_or_semipermanent_polish_for_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1800j6d</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>my index finger nail is straight instead of in a U shape (just like my ring finger) what can I do about this? and which nail shape suits me best to file? My nail polish also flakes off my fingers quickly.. And which oil/nail polish do you use for nail growth?</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1800j6d</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1800e1d</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>New to nails. Asked for short almond but these feel a little long? Is that right or do I need to just be asking for shorter?</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6u7cht78sk1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>18001zi</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Fall nails!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18001zi</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>17zzr2p</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>🐢 🐢</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g88bj4lunk1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>17zz0fa</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Cherry girlie</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b5445f0jik1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>17zyz7y</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Jasmine vibes. (credit: Myself, mods this is my own designs plz dont take it down)</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7o174y0aik1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>17zyrzm</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Tips on making gel-x last when doing it at home</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0np5c4btgk1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>17zy1qf</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Trying to perfect the glazed chocolate donut trend 🍩</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ky1bv526bk1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>17zy1h8</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>I love them!!</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zg3ulr7bk1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>17zxeo3</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>pov: i'm wild for nail art but i'm a farm veterinary surgeon 🐆💅🏻</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mql1fz4j6k1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>17zx8if</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>How to treat stained nails?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17zx8if/how_to_treat_stained_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>17zwvdf</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>zoom in for the details 🥹😍</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkk5jyvg2k1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>17zwsyh</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Chrome on top of nail art? Would it ruin it?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17zwsyh/chrome_on_top_of_nail_art_would_it_ruin_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>17zwjav</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Would this work? (Context below)</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76m3vvhyzj1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>17zvdl7</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Do you like this new set ?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/miplmdo8rj1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>17zvc7j</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Nail growing underneath top nail</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6m5ys6lyqj1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>17zuuv1</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Got my nails done for my wedding!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zuuv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>17ztc11</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Christmas gingerbread cookies🤎</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ztc11</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>17zt21i</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Thanksgiving Nails🍂🍁🤎🧡</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zt21i</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>17zs95d</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>I love long nails. What do you think?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1oq4q65m3j1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>17zs5vl</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Lead gray</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6qbrxrw2j1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>17zrz8p</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>tried pink tips for the first time</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zrz8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>17zrygm</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>More water slip decals</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zrygm</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>17zra9n</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Labradorite/Galaxy Nails ✨</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d7vt6xg2wi1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>17zpvtt</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Thoughts?🌼</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ynez36lki1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>17zog9c</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>[PR] Velvet Ribbon by ORLY 🌹</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zog9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>17zocwi</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>shorts nail</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sn5qoqt37i1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>17znr7m</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>My new bright manicure</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17znr7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>17znei2</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>did gel extensions for the first time ever! any tips or advice?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dc6rd7alxh1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>17zndd2</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Love this set. - done by me</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zndd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>17zmzov</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Should I go full sparkle?</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lfy9zn86th1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>17z7g3j</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>practicing! Vincent van Gogh inspired nails</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lw3food2hd1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>17z7hd8</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>First time getting acrylic nails.</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17z7hd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>17zjtf4</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Gel tips falling off?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17zjtf4/gel_tips_falling_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>17zhgg0</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>UV Hard Gel nails coming after only 6 days:( Is this a normal experience at a nail salon?Rant</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/17zhgg0/uv_hard_gel_nails_coming_after_only_6_days_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>180bdzy</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Help repair my damaged nails!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180bdzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>180aci5</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Halloween Color Doing Thanksgiving Duty</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6m1csl2c8n1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1809web</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Bit of sparkle from Brisbane</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ros7lhlg3n1c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1809u2j</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Two months ago I would have told you I’d never…</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1809u2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>18098s3</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Please tell me your opinions on these specific polishes (more details in the text bit)</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18098s3</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1808h8v</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Looking for a deep red jelly</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1808h8v/looking_for_a_deep_red_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>18083eo</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Help me have the courage to ask for a refund.</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18083eo/help_me_have_the_courage_to_ask_for_a_refund/</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1807rp0</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>The changing faces of teenage witch</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1807rp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1806rb1</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Had way too much fun making this glow in the dark set</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1806rb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1806hw3</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>We love a sparkly pink palate cleaner (ft my first LynB polish!)</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1806hw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1805xt3</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>The Convict (BKL)</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1805xt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1805s9h</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>First time buying ILNP polish. what should I get?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1805s9h/first_time_buying_ilnp_polish_what_should_i_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1805ou4</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Just finished these. I'm going to clean up the edges but I'm happy with it.</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fkitwwryl1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1805ojt</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Rare toddler mom manicure</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1805ojt</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>18052i7</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Gold french for Thanksgiving! 🦃</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8d2h669tl1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1804d6i</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>One of my fav nail art I have done</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1804d6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>180490z</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Light Purple Polish Recs</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/180490z/light_purple_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>18031bo</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Pour some gravy on meeeee</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18031bo</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1802z6w</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Candy cane inspired nails ❤️🤍</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1802z6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1802mzd</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Looking for Dior Vernis #997 Blue Label</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1802mzd/looking_for_dior_vernis_997_blue_label/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>18022c4</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Is there a faster way to remove gel manicure?</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18022c4/is_there_a_faster_way_to_remove_gel_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1801v6u</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>H&amp;M - Science Fiction</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1801v6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1801hv6</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>This color makes me feel things</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94kxf1y80l1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1801e3a</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>The holiday red of my dreams!</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1801e3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1800vxv</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>💜✨🩷</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1800vxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>17zzd9c</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Green &amp; Yellow 💚💛</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rj15wmv3lk1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>17zz0u2</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>cirque tortoiseshell set</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17zz0u2/cirque_tortoiseshell_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>17zx73x</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>DND Chrome Effect Powder Ingredients</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17zx73x/dnd_chrome_effect_powder_ingredients/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>17zv8i9</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Best base coat to prevent yellowing?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17zv8i9/best_base_coat_to_prevent_yellowing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>17zum7f</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>To start over or not to start over…</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/252n6chhlj1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>17zum02</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>How to stop the chipping?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17zum02/how_to_stop_the_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>17zugup</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>To the person who posted the magnet technique earlier today. Thank you!!</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bwr7591bkj1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>17zueso</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Magnetic polish Your Heart's a Black Hole</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zueso</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>17zu9nd</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Going short for a while, and trying out a fun thermal! 🍩</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zu9nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>17ztzgt</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>My acrylic nail lifted from my nail bed and I don’t know what to do</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17ztzgt/my_acrylic_nail_lifted_from_my_nail_bed_and_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>17ztkz8</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Potion Polish - Painted Sky at Dusk</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17ztkz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>17zt86a</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>A Ghost Walking Through Vegas</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zt86a</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>17zsnzq</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Finnish brand Lumene</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oymdr9pu6j1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>17zsjfu</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Last weeks set, obsessed!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f63y86rt5j1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>17zsdnh</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Blood red 🩸</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zsdnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>17zrzru</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Weekly check-in for those on a no buy, low buy, etc.</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17zrzru/weekly_checkin_for_those_on_a_no_buy_low_buy_etc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>17zryjr</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>[PR] Velvet Ribbon by ORLY 🌹</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zryjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>17zqr0i</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>{PR} Fun with Flakies 🤓</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hnntq2trri1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>17zqp1q</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Time for bright colors again</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zqp1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>17zqi2c</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>A little classy, a little festive, a little spunky to get me through this week.</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zqi2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>17zprmy</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Velvet hack success!!</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r49vz4hjji1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>17zpok4</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>My nails chip so quickly and it’s driving me mad 😫 what am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17zpok4/my_nails_chip_so_quickly_and_its_driving_me_mad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>17zmuye</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>The best polish "Rouge Noir" Chanel!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wv6x13qrh1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>17zmnqn</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>wearing holo taco „feeling fiendish“ and „polar princess“, so shimmery 😍✨</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/34aay9tiph1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>17zm72u</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Mooncat Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zm72u</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>17zm1nm</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/17zm1nm/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>17zlidq</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Yellow out there! 😁</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/tEKRBVt</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>180c0so</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>This has to be my favorite set I’ve done</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pso039q3sn1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>18080ci</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Slightly better photos…..</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18080ci</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>180308x</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>It’s timeeee!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180308x</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1800jio</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>My 1st gel</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0p3brubtk1c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>17zym2m</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Christmas Nails on myself ◡̈</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4uzut2xjfk1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>17zvog2</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Chrome without UV light</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/17zvog2/chrome_without_uv_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>17zrxl5</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>More water slip decals….</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zrxl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>17zogz5</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>long nail by me. forest colour</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/szoc17h38i1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>17zmngg</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>First time attempting nail art.</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/17zmngg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>17zmdjx</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Christmas nails done at my local salon 💜 ig@ fivestarnails.letchworth</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trhkrw9dmh1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>17zlhy7</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>First attempt at Xmas nail art</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8c9kzdhjbh1c1.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Nov 22 08:08:32 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_26.xlsx
+++ b/data/2023_11_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C427"/>
+  <dimension ref="A1:C562"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7692,6 +7692,2301 @@
         </is>
       </c>
     </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1813zgx</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Subtle gel polish on natural nails</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abyqgsc4vu1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1813uns</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Less is more ig</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytz0gbkdtu1c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1813n6t</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>First time trying brown!</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8nxqq0qqu1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1813cxv</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>New to Nails- Seeking Advice</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1813cxv/new_to_nails_seeking_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>18138h7</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>how is that?</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7xfscqflu1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>181319q</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Do these press ons look super obviously fake?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jb9jmim4ju1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1812x8o</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>mooncat - ghosts of hecate ✨</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1812x8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1810y95</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>My new nails!</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1810y95</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>180zlym</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Simple nude but I love it!!!</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqimn6egit1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>180zazr</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Bio gel overlay on my natural nails!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8qgf57pft1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>180ywch</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>got my nails done for the first time ever!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180ywch</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>180yrmd</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Airbrush cowboy baddies</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czdic8vtat1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>180ylni</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Love my new press-ons!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nusjl479t1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>180yhts</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Thanksgiving nails… I guess.</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180yhts</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>180ybo6</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Holiday Short Nails ✨</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sul1z3l6t1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>180x13i</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>🥹🥹🥹🥹❤️❤️❤️</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mjgsfzzus1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>180wuvo</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Sorry my video was so bright!! Here’s pics! Hopefully not so bright 😆</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180wuvo</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>180wmq6</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Strongest Amazon polygel?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180wmq6/strongest_amazon_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>180w40h</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Vacation nails</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/er6oluz0ns1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>180vrwl</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Nail Reddit, Help! What is this?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o8rp0tk1ks1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>180vmcq</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>I’m proud of them 💕</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aa9nlgiuis1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>180v7hq</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Let my nail artist pick my set today!</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ve4ngk8lfs1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>180u8re</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Dip set! Is square the new round?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izg4qf6v7s1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>180u84g</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>they turn matrix green when light is shown under them</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180u84g</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>180u7oc</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Still so obsessed</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnbsa65o7s1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>180u555</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>What polish did I have?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180u555/what_polish_did_i_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>180u2rz</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>My new obsession</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64ojc5nn6s1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>180tuin</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>My “utility nails”</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvorwp1u4s1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>180tjku</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Thanksgiving nails🦃💅🍂</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180tjku</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>180tj6l</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Cozy winter plaid nails</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxmwxiob2s1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>180tfi0</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Es normal que mi cutícula sangre siempre??</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180tfi0/es_normal_que_mi_cutícula_sangre_siempre/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>180ta4o</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Playing around with color pairings!</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssjgr9ie0s1c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>180t7yv</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>My Christmas/Winter nails!</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11816yjxzr1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>180svbu</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>An ode to autumn before winter descends upon us 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180svbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>180slok</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Christmas nails!!!</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbzyvdsfvr1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>180rla3</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Autumn set</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180rla3</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>180q7v5</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Why do my nails look like this?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180q7v5</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>180s1s6</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Got nails done. Went on vacation. Got broke. Now they look like this. Asking for advice!</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180s1s6</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>180rdne</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>I know it’s fall but…</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h1b6ndkjmr1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>180qwrw</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Tried builder gel for the first time! Struggling with shaping the nails</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24cmd4e3jr1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>180qtz7</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>He's sending messages xo⚘</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180qtz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>180qrh9</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>🌵🪵 mooncat's Prickly Pear and Stumped were made for each other ✨😍</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180qrh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>180qqhz</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Which configuration looks better?</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180qqhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>180q69e</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Should I cut them or keep growing them?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180q69e</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>180owrv</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>My second attempt at Gel-X!</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/724lr6cw3r1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>180n7og</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Ladies how do you take care of your right hand nails?</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180n7og/ladies_how_do_you_take_care_of_your_right_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>180ohb7</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180ohb7/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>180od86</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>gothic frenchies !</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfycs7cvzq1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>180obz7</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Winter office nails. What do you think?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180obz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>180o2u3</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Still practicing but did my winter nails today</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180o2u3</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>180njs1</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>What I need to make my own gel nails?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180njs1/what_i_need_to_make_my_own_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>180mm5a</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Any tips? 😭</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4829urg9mq1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>180m8m4</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Return Question</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180m8m4/return_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>180m6hv</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Don't mind my unpolished nails</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sq8xlbvxiq1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>180leik</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>What is your favorite nail glue?</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180leik/what_is_your_favorite_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>180lcqw</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Finally Fall 💅</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180lcqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>180l7mw</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>i work in jewellery. i was thrilled when this emerald came in</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goasrawmbq1c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>180l3wb</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Advice for strengthening natural nails?</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180l3wb</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>180kts5</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>New nails 😊 !</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eec4zloo8q1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>180kc17</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Happy almost turkey day ! 🦃</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lefjg79s4q1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>180k2fe</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Thanks for the advice for proposal nails, I went with the pink and have no regrets! 🥰</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pejjhyr2q1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>180jvk3</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Rainbow nails, so colorful</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180jvk3</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>180jgns</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grey Nail Polish deserves love ❤️ </t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/933lqpx1yp1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>180irw7</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Nail kits for 10 year old</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180irw7/nail_kits_for_10_year_old/</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>180iebi</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>🫣My Attempt At Russian Almonds 😅🩷</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180iebi</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>180idcg</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Advice on how to keep gel extension tips SHARP?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mydk0w9dpp1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>180huks</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>What is the difference between press on tips and gel x tips?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180huks/what_is_the_difference_between_press_on_tips_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>180gxla</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>PSA: Dior Creme Abricot now 8g</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldqrmf05dp1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>180gqze</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Just started doing my own gel nails in October 💅🏼</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180gqze</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>180fs3o</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>New nails 😇🥰</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvq7ie382p1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>180euno</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Gel with a tip?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/180euno/gel_with_a_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>180edfi</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Started doing my own nails recently, what do you guys think? :)</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ssgorlfmo1c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>180e9c2</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Subtle little holiday 🥰</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/whr87810lo1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>180ds69</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Did I do okay ? Gel tips with gel glue and I used light pink builder gel on top e filed then cow print . So far they’re on nice n tight .</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180ds69</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>180cbwf</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>My nails are in horrible condition</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180cbwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1812myj</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>International shipping—mail forwarding service experience?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1812myj/international_shippingmail_forwarding_service/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1812j92</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Holo Taco Linear Holo Top Coat 😍</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1812j92</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1811g2q</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Mooncat - Ghosts of Hecate</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1811g2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1810d2q</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Subtle and Glowy</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j7cszzqtpt1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>180zwda</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>With real err.. OREGANO encapsulated.</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8qa7nu7lt1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>180z7nt</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Totally swamped with studying, and chewed my nails off from stress. Finally took the time to do some self care.</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8lhkacwet1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>180z1ni</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>todays mani :3</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyrsyvkddt1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>180yozv</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Not great lighting but my pink nails to go with my pink flamingo quilt that I'm working on</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rr117as2at1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>180y921</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Zoya Haul - ordered Nov 11</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93p7nzdx5t1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>180y64l</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>My winter nails have done!😊❤️</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vfxm0y55t1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>180y027</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Subreddits for frankenpolish/diy?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/180y027/subreddits_for_frankenpolishdiy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>180x70i</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Inner cap replacement?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://ibb.co/MVMDqhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>180wka6</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Full Blast</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180wka6</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>180w3xu</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>I just love how cozy yet sparkly this color feels ✨</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2x3qm20ns1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>180v375</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>pastel holiday colors I guess?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tuterr0mes1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>180uc28</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>does anyone know what these annoying lines are and how to get rid of them? i really want to do sheer polishes but can’t 😭</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47psamdk8s1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>180tud0</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>winter wonderland nails ❄️⛄️</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/720kuqct4s1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>180tsn4</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Thanksgiving mani with subtle stamping.</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv83byrf4s1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>180tqwq</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Looking for an icy blue to lavender shifting color similar to this combo</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjzjxmz14s1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>180tm36</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Can I use OPI Infinite Shine 2 with any base coat?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/180tm36/can_i_use_opi_infinite_shine_2_with_any_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>180tkq5</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Has anyone’s 10 for $25 Zoya polishes sale orders actually shipped yet?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/180tkq5/has_anyones_10_for_25_zoya_polishes_sale_orders/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>180tcqm</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>mooncat - mad hatter</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180tcqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>180t079</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>ILNP is trying to get me</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/180t079/ilnp_is_trying_to_get_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>180srh3</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>HT’s Sunken Secrets v ILNP’s After Midnight</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/180srh3/hts_sunken_secrets_v_ilnps_after_midnight/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>180roly</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Thanksgiving Nails🦃</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180roly</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>180rkx6</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Need help finding a dupe</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0fe1lpi0or1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>180rcjc</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Millenia 🧲🌌</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180rcjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>180qpoh</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>🌵🪵 mooncat's Prickly Pear and Stumped were made for each other ✨😍</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180qpoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>180q29z</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>They were hella messy but this was my Halloween set!</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180q29z</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>180pmf9</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Fallish Rainbow Skittle</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0s3uqka9r1c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>180oid8</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>1st gel</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65cq42ax0r1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>180pb21</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Love the glitter “french mani”!</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqzyqlfv6r1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>180ozdr</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>My solution to the little problem</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3imphghg4r1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>180okyu</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>I’ve never seen this product mentioned and I love it for growth!</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g8ppduf1r1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>180o2wk</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>My boyfriend tried to do my nails 😭</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7du46hqxq1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>180o2cf</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Matching nail polish?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uneeelrlxq1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>180o0n7</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>A perfect green + first glow in the dark!!</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180o0n7</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>180mshv</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>The one mani you can’t take off</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xi4tfgrmnq1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>180mgi7</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Dupe for OPI Black Dress Not Optional?</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/180mgi7/dupe_for_opi_black_dress_not_optional/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>180k9pq</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Baby's first black mani 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q58ndlyc4q1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>180k75y</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Mooncat House of Hades and my first Legos set</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o67avovs3q1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>180k2ce</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Just finished doing my nails and noticed that one hand is darker than the other. How do I fix this!?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/180k2ce/just_finished_doing_my_nails_and_noticed_that_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>180iz24</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Nails are Thanksgiving ready!</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9epg5wy8up1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>180hzkw</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Tips for making nails last longer?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/180hzkw/tips_for_making_nails_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>180hq11</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Help! Marks on my mani every time.</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jlk0hqwwjp1c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>180g8zi</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Any PA,NJ,NYC Laqueristas want to team up for ILNP or Zoya haul?</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/180g8zi/any_panjnyc_laqueristas_want_to_team_up_for_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>180g5vw</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Peeling nails - help please!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blvzb9f06p1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>180ei2f</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Finally learnt to not flood my cuticles</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lv2snyxno1c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1803mzq</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>My male painted toenails. Always have them painted and change the color every two weeks.</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1803mzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1812qpw</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Name of this technique/product - what do I search for?</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep8pegbnfu1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>180wpgw</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>I know it’s fall but…</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwpavv66ss1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>180to3f</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Tried doing cherry blossoms</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqdhntve3s1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>180rnbz</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Autumn set</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180rnbz</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>180ojtw</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>My take on office nail for winter, practicing doing tweed pattern. What do you think?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/180ojtw</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>180nsgt</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Rose red with sparkling diamonds</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s257zr35vq1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>180joc9</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>hhh how they look</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/180joc9/hhh_how_they_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>180hve3</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>New to gels and nail art, and I'm trying to practice every day. Here's day 34</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ptn1iv40lp1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>180g54x</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>new uv-nails :) did them myself :)</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lwicvlfs5p1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>180e3xo</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Basic, but first time I do it myself</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/duiboik2jo1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>180dnkc</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Simple nude with gems</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qt754ib3do1c1.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Nov 23 08:08:16 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_26.xlsx
+++ b/data/2023_11_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C562"/>
+  <dimension ref="A1:C711"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9987,6 +9987,2539 @@
         </is>
       </c>
     </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>181w4a7</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Tips for double lining french?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/181w4a7/tips_for_double_lining_french/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>181vdh1</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>My spin on holiday nails ❤️</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v10o20iiq12c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>181vdau</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Nails look bad underneath?</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181vdau</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>181v9pe</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Subreddit was right, glossy taco really brought the press tons together (gonna make the tips a lil more symmetrical though)</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181v9pe</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>181v5o8</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>I'm ready for festivities! Did I do the press ons nicely?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvnzlam0o12c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>181tr5l</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Bro excuse me? I LOVE polygel omg</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy1jipsf812c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>181sgy9</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>I tried to do these a year ago and failed miserably</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181sgy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>181rxjf</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Sailor Moon inspired 💝✨</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181rxjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>181iql3</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>How do I remove my press on nails when I want to reuse them?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2zjfpkpky1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>181inc2</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>How do you entertain yourself while doing your nails?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/181inc2/how_do_you_entertain_yourself_while_doing_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>181gm8d</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Why do my nails ALWAYS look grown out a couple days after getting them done?!</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181gm8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>181rvyr</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Natural growth tips?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/181rvyr/natural_growth_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>181rou7</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Clear rubber base gel in Australia?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cre56hzm02c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>181rk4z</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>🤎🍁</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5bvt3ypl02c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>181rjyf</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Went Chrome neutral for thanksgiving. Love them.</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xjv3s7ol02c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>181r24d</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I tried 😆 not bad though for my first grinch ever! 🥰 </t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0ywfexp3h02c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>181r2hn</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Simple but soooo cute!!!!</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mzqkdiv7h02c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>181qre5</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Since a lot of ppl like my husbands nails, I decided to do them too!</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7kslmcce02c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>181pmxw</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Purple tulips ? What do you think they look like ?</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181pmxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>181ospy</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>First Set of Gel X Nails 🧡🖤🩶</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0l6ysa4cwz1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>181osix</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Is there a stencil or guide to help shape nails?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/181osix/is_there_a_stencil_or_guide_to_help_shape_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>181np4y</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Cranberry sauce nails 🥰</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/emdl37ztmz1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>181nhz6</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>First time wearing nails 💅🏽</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181nhz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>181ndqd</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Matte black &amp; gold 🖤💛 should I switch to brown for Thanksgiving tomorrow?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181ndqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>181n4bs</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>3D rose nails</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181n4bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>181my6j</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Cotton candy swirl nails!</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9afuzqemgz1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>181mdh0</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Nail dust collector??</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/181mdh0/nail_dust_collector/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>181lwu9</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Accent nails 🥲</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3dj6ggk8z1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>181l4ow</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Builder on natural nails keeps breaking</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/181l4ow/builder_on_natural_nails_keeps_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>181klqo</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>I got extra long so they would cover my nails and they still don't!</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181klqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>181k6vw</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>DIY mani 🪩</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181k6vw</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>181k6tv</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Trying a new shape rather than just almond</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25qb3diovy1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>181jzia</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>I let my nail tech decide the shape and style this time</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181jzia</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>181jzcc</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>My journey with biab. Cuticles looking crusty.</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181jzcc</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>181jxxm</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>3D Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8nyqvqqty1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>181jhn4</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>For the long nailed girlies - must have things/methids to help with every day activities?</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/181jhn4/for_the_long_nailed_girlies_must_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>181j306</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a14ccpheny1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>181irjg</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Hypnotized by this pink 💕</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7njm5u4xky1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>181ig4q</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>This week nails</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04e7ihzdiy1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>181ieux</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Too early for Christmas nails?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/os2szi44iy1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>181icjx</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>My best friend has the most perfect hands 😍</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181icjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>181hdy0</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Hand Sculpted/ hand painted Thanksgiving dinner nails</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181hdy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>181guzc</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>My latest set vs earliest set</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181guzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>181g93b</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>should I shave down the hearts and do all pink chrome? Gel x I just did on myself and I think I hate the hearts! Thoughts?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/di8c70gh1y1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>181fny1</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Got these done yesterday ☺️🌺</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181fny1</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>181fj25</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Love my new nails ✨♥️👀✨</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181fj25</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>181f5pp</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Ok nail peeps. I'm still swatching. I currently have all my pigments separate from my polishes as they are a powder and I'm thinking of swatching them as well and now I'm thinking should I mix the pigment container in with my other colors or still just leave them separate.</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181f5pp</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>181f2ru</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>My new obsession ♥️</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181f2ru</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>181ere9</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>✨❤️🧡🤎HAPPY THANKSGIVING!!✨</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181ere9</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>181elnr</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>I always find it attractive that they look simple what do you think?</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8m9ptf88px1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>181egw9</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Close up on these pretty nails! I’m obsessed 💗</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/baz3k4u8ox1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>181e9aw</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Alien nails are my favorite nail genre</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181e9aw</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>181e6q8</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Still practicing, and still gotta clean up on the edges, BUT LOOK AT MY EARLY CHRISTMAS SET! (Last pic is my right hand and was way harder).</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181e6q8</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>181e37m</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Just had to cut down my natural nails, opted for this maroony red, love this cat eye!</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56cyjws9lx1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>181dhgn</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/181dhgn/christmas_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>181ddf3</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Anyone go from acrylic to press on?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/181ddf3/anyone_go_from_acrylic_to_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>181daac</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Full set</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v210fte2fx1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>181dhdh</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>🎀</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydb7yalmgx1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>181c946</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Simple White on White for the Holidays</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181c946</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>181bv3m</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Unsure about this set</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181bv3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>181bdrx</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>It's such a gift to be nail tech! You can do any nails for yourself, in any day :) But doing right hand it's really crazy</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181bdrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>181awtf</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>When my husband lets me practice on him :)</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylc9lu6uxw1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>181akeo</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Black Aura Nails with sparkles and Holographic Butterflies IS A VIBE ✨</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8pqxmruvuw1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>181a6at</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>More amazing nail art by Minea</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5vgtmkgrw1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1819suq</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Glittery red for the holidays</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1819suq</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1819mtw</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Love my new nails😍✨⭐️</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1819mtw</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1819hcj</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Holiday nails!</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1819hcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1819egi</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Thanksgiving/autumn mani</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mco9wn1zkw1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1818341</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Most Lavish Set Yet…</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1818341</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1817w1p</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Fresh 💅</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9l2lidk6w1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1816n76</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Thanksgiving mani 🦃</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1816n76</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>18152hq</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>First time shaping my nails, how did I do?</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18152hq</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1814cbj</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Star nails !!!</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihr7qgugzu1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>181uwqx</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Velvet mooncat smokescreen!</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nmteu858l12c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>181un2h</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Thank you for the velvet hack!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkdnfls9i12c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>181t41o</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>My experience doing velvet nails with the hack vs. the “long” way.</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9y0bi3rl112c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>181suv0</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>We'll be hanging out at the relish tray on thank</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1flc97xy02c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>181sqo8</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>ISO A Gunmetal Blue Polish. Any recs?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/181sqo8/iso_a_gunmetal_blue_polish_any_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>181sl60</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>How does this nude look on me? With and without flash on for comparison.</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181sl60</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>181r39k</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Glowing Without Blacklight!</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5onvo9pfh02c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>181puyk</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>House of Hades</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181puyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>181pt68</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Pearl Jammin' in sun and in clouds</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181pt68</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>181pki0</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Flaky Carrot Cake</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fi7afec302c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>181p8az</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Was going for a fall vibe 🍁</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djj3if38002c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>181o776</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>I like the turn out, but does anyone else?</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff9de6r1rz1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>181nsj5</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Midnight Mantra ✨️</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8ayerrknz1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>181n2dt</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>How does one achieve this magnet look?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181n2dt</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>181mre0</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Can’t stop staring at the sparkles!</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r52gazi3fz1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>181mmuj</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Tried Olive &amp; June polishes for the first time</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ivj1os2ez1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>181m134</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Thanksgiving manicure</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlrh0lbf9z1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>181lpff</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>[Polish] House of Hades by Mooncat: opacity swatch comparison</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://imgur.io/a/eSKZ1IO</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>181ll4r</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Thanksgiving nails</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssiy6ru26z1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>181lfqx</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Thankful for this Sub</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/181lfqx/thankful_for_this_sub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>181l92q</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>New mani to get me out of my feelings</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181l92q</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>181l90v</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Shimmery Ethereal mani</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gz3c93ef3z1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>181kxlr</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>First time using DND gels</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5pu8dpx51z1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>181k8y2</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>DIY mani 🪩</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181k8y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>181k2jp</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>On today’s episode of “the swatches are lying”…</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181k2jp</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>181jplh</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Mooncat Mad Hatter (velvet trick)</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/otgp7ebzry1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>181jbmd</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>SYS - Weekly Challenge #2 - Something epic</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/waitoa28py1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>181j9n5</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Tiffany Inspired Nail Art</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0iaaz9asoy1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>181j956</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Mooncat Tyrannosaurus Hex</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181j956</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>181iy38</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Guess who accidently put a deep red brush in my top coat?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4m0iryi5my1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>181ipwb</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>What’s my undertone?</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181ipwb</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>181hwpx</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>I'm outgrowing my organization! Does anyone have one of those spinning tier things? Do you like it?</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181hwpx</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>181hda5</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Ready for Mario Kart tournament !</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181hda5</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>181h0pk</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Witchcult's Guardian Angelfish</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181h0pk</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>181gkol</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>ILNP-Penny</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edlc7jhx3y1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>181ggzg</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Enjoying the last bit of fall</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181ggzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>181gfzq</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Mooncat’s A Midsummer’s Dream… painted by my amazing husband!</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181gfzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>181ftxj</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Essie “Berry Naughty”</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojzd55fcyx1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>181fgeu</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Shy rainbows</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181fgeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>181f10s</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Sand Viper day 7 and help with neutrals</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhzimv5csx1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>181eugs</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>✨❤️🧡🤎HAPPY THANKSGIVING!!✨</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181eugs</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>181eezy</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>I couldn’t resist this color! It’s gorgeous!</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/luxgug7unx1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>181e8iv</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Question about Essie and general advice needed</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/181e8iv/question_about_essie_and_general_advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>181deo1</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>In love with this color</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zt2f1220gx1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>181dema</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Are topper skittles a thing? Topper skittles should be a thing.</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2xyjio8nfx1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>181cy9k</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Used some Aurora tape and chrome powder for a very shiny, shifty mani</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181cy9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>181cumi</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Just a little bit festive…</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qpm6djqbx1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>181cugw</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>'Polishes I Never Use' part 2 😀</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/MzJiTQ7</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>181cl50</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>{PR} Ok just 1 more photo… 😍</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jt5y57fz9x1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>181cjix</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>On the Solar Train</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181cjix</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>181bkvu</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Mooncat is worth the cost</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181bkvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>181amfh</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Why are my nails bumpy like this? 1 coat basecoat, 3 coats Mooncat A Midsummer's Dream, 1 coat topcoat</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mghukt8dvw1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>181a4gz</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Any tips for being neat with gradients? Twilight Stardust mani (forgive the mess, I’m learning 😅)</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jssrani0rw1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1818bcx</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Pumpkin Pie</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qm2lowxaw1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>18183bs</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>I’m a jelly addict now 🫣🤫</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18183bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1816ix1</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Thanksgiving mani 🦃</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1816ix1</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1815vsp</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Mooncat’s haunted forest</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6q7k5ewbjv1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1815l14</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Help me find a dupe for the best COOL TONED LIGHT PINK JELLY ever!</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1815l14</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>181w6sz</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>My nail for winter, what do you think?</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akgn7qv3022c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>181vnge</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Nails done by "Nails by Gen" 💅</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wliki9vvt12c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>181uu1b</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Made Press Ons</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/komh73nfk12c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>181tdeb</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Merry christmas🎄🎄</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zded77h412c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>181t0mh</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Holiday practice nails</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqvcvhfn012c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>181snf6</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ytubw6qw02c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>181shz2</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>I failed miserably at these a year ago</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181shz2</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>181rqvf</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Mmm. Gingerbread!</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ag0p7cjn02c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>181qsv0</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>My daughter’s birthday set!</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dou8xzdqe02c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>181nr6u</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Cranberry sauce nails 🥰</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tgo7ualanz1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>181nftb</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Just finished 🙂 thoughts?</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0v92m6mkz1c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>181ih7a</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>This week set</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuhwdtumiy1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>181fg9o</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Azure Beauty Dip Nail Extensions / A Very Blingy Fall</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://youtu.be/VzfWybsxngE?si=qThlxziARpCQPkC4</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>181ebyn</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>chocolate chrome 🤎</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qpeyccf6nx1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>181dftz</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>🎀</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0kj2azo9gx1c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>181b402</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Fairy core ✨</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181b402</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>181amrs</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Black Aura Nails with sparkles and Holographic Butterflies IS A VIBE ✨</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9ar0rpsgvw1c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>181a0fy</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Candy cane nails :)</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181a0fy</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Nov 24 08:08:33 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_26.xlsx
+++ b/data/2023_11_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C711"/>
+  <dimension ref="A1:C819"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12520,6 +12520,1842 @@
         </is>
       </c>
     </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>182mqns</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Obsessed with how much these press-ons matched my purse</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bqgzmije192c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>182lmlz</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Red nails for winter season❤️</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmyxfq91p82c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>182llws</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>I’m so glad I learnt how to do my nail’s myself</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182llws</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>182lee0</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wz8qgbjm82c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>182kxtv</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Thoughts about my nails design?</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2x3g1uoph82c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>182k54p</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Lil funky brown look</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyk46uoz982c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>182j9a3</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182j9a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>182c1of</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Anyone have any Healthy Natural Nail Tips?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182c1of/anyone_have_any_healthy_natural_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>182ib8p</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Men with painted nails</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182ib8p/men_with_painted_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>182b8x6</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Still can’t get over my Nezuko inspired set</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182b8x6</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>182amlb</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>BIAB ruining my nails?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182amlb/biab_ruining_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1827i00</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Weak nails and press-ons?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1827i00/weak_nails_and_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>182604g</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>New party nails for the season</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182604g</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>182hk3s</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Velvet Nails</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4ll04ofbk72c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>182h6hf</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>What made you stick to regular polish?</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182h6hf/what_made_you_stick_to_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>182goup</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>From several months ago but my tech is amazing</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nngz9w4c72c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>182g1br</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Some subtle fall nails for Thanksgiving</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p84jex5w572c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>182fu2k</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>What do you guys think? Do they go well with the look?</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9gefv6kt372c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>182fgdp</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>First time doing my own</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182fgdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>182eq4u</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Which length do you prefer?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mjbn4zit62c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>182e9jg</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Gel-X tips</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182e9jg/gelx_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>182e3h8</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Is this length of polish-free nails grosss? I’ve been very busy lately and doing my nails have been pushed to the side</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182e3h8</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>182dwoe</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Absolutely in love with my nails</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182dwoe</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>182djb8</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Looking for a winter look</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14ck3jw4j62c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>182cjk4</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>How to Shape</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182cjk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>182cd9w</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Some florals giving summer vibes for vacation 🌸</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182cd9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>182c88p</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Happy Thanksgiving!</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182c88p</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>182bd0c</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Stop Using Gel!!!!</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182bd0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>182b0j9</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Need help finding nail related Christmas gifts for mom</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182b0j9</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>182anil</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Day of giving thanks!!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182anil</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>182am1z</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Trying acrylics for the first time. helpppp</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182am1z/trying_acrylics_for_the_first_time_helpppp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>182akht</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>My girlfriend has the best and cheapest nail tech. She’s always excited after her nail appointments to show me what she’s got done. (The last two pictures are a screenshot from a video.)</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182akht</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>182808y</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Can I mix gel polish and acrylic nail polish?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182808y/can_i_mix_gel_polish_and_acrylic_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1827xfl</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Just for fun, spotted on IG</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qv7bodf8752c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1827viq</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Ice Queen Claws</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmgnsfys652c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1827kw9</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>The latest set, haven't done ombré in a while</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1827kw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>18276uu</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>I love this shade of blue so much</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aechzjd4152c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1826srh</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Russian Manicure Question</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1826srh/russian_manicure_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1826l2q</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>From a scale of 1 to 10 how christmasy is this set?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1826l2q</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>182670q</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Ballet slippers, iridescent chrome, clean cuticles ✨</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182670q</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>18265g3</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>I don’t celebrate thanksgiving, just here for the food 🤎</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uy2dh4o5t42c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>18251r9</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Darkness and ice</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lq7fnbuck42c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>181yztt</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>2nd time doing Acrylics on myself, need a lot more practice... But I'm happy with em</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181yztt</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1824x3y</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>what do we think of this color? too much?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1824x3y</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1824sbt</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>First gel-x fill</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1824sbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1824qcq</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Shiny nail cuticles normal?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1824qcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1824jji</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>I have been obsessed with chrome lately!</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tdw46s3ag42c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1824j0k</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Thanksgiving nails!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qt96svb6g42c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>182406w</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>HAPPY THANKSGIVING 🦃</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182406w</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1823i51</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>What would you call this art?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3avk37hu742c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1820fru</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>I'm a sucka for sparkles</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1820fru</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>181zmgg</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Fall jewel tones with matte/ shiny French</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrqb01dz632c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>181yy3b</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>First time with new technician!</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181yy3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>181xu1x</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>New to nails</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/181xu1x/new_to_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>181x3wv</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ra2kdx6xb22c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>182mjdt</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Dazzle Dry coupon link ($20 off $65)</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/182mjdt/dazzle_dry_coupon_link_20_off_65/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>182lyn8</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Tried something new! Branching out from purple 😂</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/byg7gysls82c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>182lm93</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>First Sassy Sauce haul!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0e1jge8xo82c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>182kpzo</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Looking for a more opaque nail polish (that needs less layers)</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/182kpzo/looking_for_a_more_opaque_nail_polish_that_needs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>182kcun</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>KBShimner, Orly Sec N' Dry and Essie Gel Couture top coat comparison reviews</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/182kcun/kbshimner_orly_sec_n_dry_and_essie_gel_couture/</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>182jbt1</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Calm before the storm</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182jbt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>182idem</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Holo Taco Sonic Unicorn Skin 💙</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsw4y9l6s72c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>182ias9</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Stoneware Thanksgiving Mani</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6flkupgr72c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>182gkrp</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Some subtle fall nails for Thanksgiving</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p3nazge1b72c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>182g48f</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Thanksgiving Manicure</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r695apdo672c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>182g3hm</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Sally Hansen INST-DRI | Zip Wine|# 428</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182g3hm</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>182fqn4</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>ILNP You Up? A midnight blue fave.</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2b9xwh1372c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>182f773</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Mooncat sales &amp; recommendations</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/182f773/mooncat_sales_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>182e3nv</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Zoya Eradani</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7e2wxq51o62c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>182di5i</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Thanksgiving Mani</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182di5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>182d9zs</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>First time trying press ons</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w4rgfxzg62c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>182b7yi</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Thanksgiving Mani 🦃🧡✨</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182b7yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>182aw2c</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Emergency manicure at my boyfriend’s sister’s house with no acetone, no base coat, no cleanup brush, and borrowed polish. It’s a thanksgiving miracle!</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1bi33zpw52c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>182aukq</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>My Thanksgiving Polish</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oepxpt6dw52c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>182agn6</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Why are my cuticles always dry and peeling?</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kn1sa1h3t52c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1829rwj</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Best ilnp Multi chromes?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1829rwj/best_ilnp_multi_chromes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1829otj</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Yet another "velvet nails magnet hack" post because OMG WOW</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f2b37xd7m52c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1829jmy</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>home for thanksgiving because covid nails</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1829jmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1829ewx</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Mall Crawler is a color that has always been on the back of my mind after seeing it here 🩷 So happy I finally grabbed it! Are all the Expressie colors this smooth?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1829ewx</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>18292k4</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>I love how dreamlike this looks</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smhxfy1wg52c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1828j34</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Thanksgiving Skittle</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1828j34</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1828890</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Hidden treasures: Trend It Up - Moonglow 010</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1828890</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>182862a</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Thanksgiving mani 🍁🍂🦃</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182862a</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1827uz0</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>{PR} Home for the Holidays Collection by ILNP 💕</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1827uz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>18276es</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Is it even possible to not love this shade?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4t1xi7z0152c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1826kpv</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Goblins and Ghoulies!!!</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1826kpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1826eqc</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Took the classic nap after painting that ruined my nails</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrdozp85v42c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>18265u7</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>My first LynBDesigns polish 🥰</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18265u7</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>182564i</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Simple yet timeless for thanksgiving</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3epbm49cl42c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>182599q</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>“In the future, everything is chrome”</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182599q</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>182574a</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>My favorite fall shade in my collection! 🧡</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w93p54fkl42c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>18255cb</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Having a Christmas themed baby shower on Saturday, decided to get festive</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18255cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1824peq</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>ILNP Shimmers</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1824peq</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1824dlo</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Pass the cranberry sauce please 🦃</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1824dlo</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1823zng</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Chrome chipping one day later. How can I fix this?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1823zng</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1823oza</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>In love with my seasonal jellies!</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1823oza</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1822df2</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Thanksgiving mani!</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1822df2</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>182339i</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Gobble gobble!</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182339i</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1822gw9</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>2 coats worked for me!</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hozsm6g1z32c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1821m4x</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Can I see everyone’s Thanksgiving manicures?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2wv3gc7dr32c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1821gn3</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Silver on black?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zyeehbqup32c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>181xrk2</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>For all the funky green lovers out there</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/181xrk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>182jluk</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Piglet’s Version</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gdxst7m482c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>182ho5o</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>My first 2 attempts at nail art</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182ho5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>182b43x</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>The Grinch of Christmas 🎄💚</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bsy1dtxiy52c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1829c42</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Icicle nails</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0j8z8d15j52c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1826llx</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Freehand design</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4uxl02ew42c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1826hv4</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Nail art practice day 36. Straight lines are tough!</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1uls2piv42c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Nov 25 08:07:14 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_26.xlsx
+++ b/data/2023_11_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C819"/>
+  <dimension ref="A1:C943"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14356,6 +14356,2114 @@
         </is>
       </c>
     </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>183e7tw</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183e7tw</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>183dgzm</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Do you need acid free primer and ph bond?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183dgzm/do_you_need_acid_free_primer_and_ph_bond/</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>183bne5</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Olive and June Press Ons in "Hz" and two layers of Goldfish Pink with a layer of Long Lasting Top Coat! Love :)</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7gbmj2olaf2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>183b3dp</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Nail bed growth/reattachment - should I try builder gel?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183b3dp</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>183b2n9</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Most desperate thing I’ve ever done in a pinch… 😬</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iguhspkn4f2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>183b24i</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Sparkles and rainbows!</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44atd96i4f2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>183alm3</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183alm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>183ah6v</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>How polarizing kb shimmer</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xo52303qye2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>183a72d</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Nude glitter with peeking pink tips 💞</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2qz61205we2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1839x7c</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>my 🍂fall🍂 set - thoughts?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6jn9v9nte2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1838xzv</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>my latest design in soft gel</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxtj3tsxke2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1837cz6</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Slip layer</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1837cz6/slip_layer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1837c9s</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Proud of my Thanksgiving nails</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1837c9s</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>183722k</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Holiday Classy Quirky</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183722k</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1833ye1</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Newbie issues with taking gel polish off</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1833ye1/newbie_issues_with_taking_gel_polish_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>18303ji</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Does this color go well with my nails and hand shape?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wrpedpulc2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1836tf0</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>The longest I've ever gotten my nails! Christmas is hereeee</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ft5k92gq2e2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1836ohg</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Tried something girly</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6o6jm2n1e2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>18367mo</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Real nails with hard gel overlay</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18367mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>18366sv</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Black and red, love it</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18366sv</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1835t2i</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>New Set On My Friend</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kaob3parud2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1835j1l</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Wet’n’wild drugstore for the win</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sycwd27jsd2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1835epo</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Longest my natural nails have ever been.</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnmaxnulrd2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1834wlp</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>I’m a big chrome fan</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1834wlp</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>18344ez</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Ending the month with a very risky new nail color, I have tried several different styles lately🤭</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iw9bs13nhd2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1833we2</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Manicure 💅</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odn4ukgufd2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1833ua3</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Chrome Finish FTW</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wcpjgaudfd2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1833u6t</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Gel manicure chipping on day 1?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1833u6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1833c2i</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Autumn set I did with red chrome underside</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7fiyeh7fbd2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>183381e</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Best top coat for long-lasting glassy look?</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183381e/best_top_coat_for_longlasting_glassy_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1832t99</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Pleasantly surprised by these press-ons!</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1832t99</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1832mg5</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Ho Ho Ho</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6wbt1uv5d2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>18329i9</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Glow in the dark Christmas lights 🎄</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18329i9</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1831pbx</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Tried my hand at the Sweater Nails 💅 Look. Need to get some acrylic powder for the 3D effect.</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6yvbh6kryc2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1831kt1</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>The season is creeping in</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/php533srxc2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1831hun</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>short nails</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8kxaur4xc2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1830wg9</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>What is wrong with these nails?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yuvrku19sc2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1830b41</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Nails today</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1830b41</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>183047i</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Got some chromes to try out. Thoughts?</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183047i</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>18301y2</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>🎄Christmas nail art🎄</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14wi0m8glc2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>182zu1c</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Press-On Peeps…what’s your favorite adhesive?</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182zu1c/presson_peepswhats_your_favorite_adhesive/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>182zi7s</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>early bday nails i just did 🎀🖤🫶🏼 (press on’s!)</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182zi7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>182zdgf</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Tried dark aura nails with eyeshadow!</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182zdgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>182ytki</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>eevee nails with pink to match her blush 🥰🤎🩷</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182ytki</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>182ocps</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>help? nails look goofy with extensions</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182ocps</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>182ocab</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Love this set, inspired of Pinterest</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32ear86wk92c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>182x4h3</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Top coat over 3d nail stickers?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182x4h3/top_coat_over_3d_nail_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>182wvd5</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>is there a reason my nails grow like this?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182wvd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>182vup1</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Glitter nails</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182vup1/glitter_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>182vooh</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>First set of festive nails</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/728gr7bjmb2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>182v4mm</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182v4mm</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>182ur3r</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Cotton Candy Chrome 💗🎀</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182ur3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>182unch</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Tis the season</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fupbosd6eb2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>182t44e</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>I miss having my nails painted so much 😭</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ke5hfnob1b2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>182syop</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>My first french manicure! Am I late to the party??</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wuhftrwyza2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>182s8ah</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Best nail glue for children's press-ons?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182s8ah/best_nail_glue_for_childrens_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>182rcgs</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Back when I used gel nail stickers…</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3bj7zd5vka2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>182qs49</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>new at doing gel + acrylic nails</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/182qs49/new_at_doing_gel_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>182qpkx</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>natural nails💕</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182qpkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>182qhbr</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>What did I do wrong? And how to fix?</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkvm2tbjba2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>182qa5o</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Do my nails look good?</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s61olq369a2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>182q4sz</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Some goth vibes</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182q4sz</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>182ps3z</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>I love to use stamping to let the gel manicure look different every couple of days</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llcchr343a2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>182pjzq</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Two big events; my first two gel-x extensions</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182pjzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>182oszj</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>My best yet manicure and design from my friend who is an aspiring nail artist</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxuiiiy2r92c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>183ev4m</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Would this be possible?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/183ev4m/would_this_be_possible/</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>183cvnm</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Tried the velvet hack...</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z9zmiyknnf2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>183ct5b</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>my second ever gel-x nail set, need some tips !</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7141t3vmf2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>183bcmk</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Am I drunk or did the Dior Abricot (blah blah blah pretentious nonsense) make my nails look amazing?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to0dgzkh7f2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>183b6fo</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>New polishes to while I grow out acrylic damage</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183b6fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>183b55d</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>There is no photo that can do this polish justice</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183b55d</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>183ah16</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Fuck these brushes tho</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183ah16</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1839llm</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Just lying in bed, staring at my nails.</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1839llm</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1839fdd</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Glittery, shimmery, icy periwinkle for the first “winter” mani</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omzg8756pe2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1838dud</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Today's Mani</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1838dud</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1838bl6</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>1st Indie Polish</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1838bl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1838201</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>So proud of how clean these Frenchies turned out!</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vtsuhr68de2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>18357ms</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Lost boyfriend seeking wisdom.</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18357ms/lost_boyfriend_seeking_wisdom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1834ntr</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Anyone know a dupe for sally hansen “go garnet?” It’s a deep blood red, almost appears black.</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eusa43k0md2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>18343ux</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Practising hand painting🦋</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18343ux</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>18341ry</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Gates of Hell 🔥</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18341ry</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1833upt</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Late to the Glass Frog party</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1833upt</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1833qpv</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>making my way through my mooncat haul 🐉✨</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1833qpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1832s39</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Mooncat Dragon Scales 🐉 love the purple green gold shift.</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1832s39</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>183283j</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Regular nail polish artists?</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/183283j/regular_nail_polish_artists/</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1831x0y</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Please help!! Is there any way to recover my vertical nail split?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1831x0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1831odf</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Clionadh October Mystery Lacquer 2023</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1831odf/clionadh_october_mystery_lacquer_2023/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1831l2f</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Nude and gold</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fqoueb4uxc2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1830uvk</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Ethereal Latte Cloud dupe?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1830uvk/ethereal_latte_cloud_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1830ejt</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Water Marbled Nail Art</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1830ejt</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>182zhsh</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>First time trying dark aura nails!</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182zhsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>182zhk7</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Magnet for the "velvet" hack</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182zhk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>182zaez</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Wow, INLP wins this sale round over Zoya</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/182zaez/wow_inlp_wins_this_sale_round_over_zoya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>182yr5z</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Looking for reviews on gel polish's</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/182yr5z/looking_for_reviews_on_gel_polishs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>182y302</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Sabertooth on a snowy day</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88v0x6fp5c2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>182xzgr</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>L.A. Colors - Ravishing Gown</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/liaud6sv4c2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>182xmhh</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182xmhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>182x24w</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>loving this combo 💓</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182x24w</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>182x001</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Pansy Flowers</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182x001</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>182wlhx</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>What’s a mess free alternative to nail oil?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/182wlhx/whats_a_mess_free_alternative_to_nail_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>182w923</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Matte ombre/gradient. This mix of colors really makes me happy!</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182w923</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>182volp</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Splurge for Dior but not really worth it</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04ri9vijmb2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>182v6os</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>New to nail salon polish</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xd4zzpmib2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>182uz22</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>It's officially red glitter szn 🎄</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182uz22</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>182uyh3</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Has anyone had an issue with ILNP coupon?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/182uyh3/has_anyone_had_an_issue_with_ilnp_coupon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>182ut0r</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Edward, desperado under the stars</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182ut0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>182uro9</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Orange and pink mani</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvdu9uc5fb2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>182uqbc</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Subtle Holiday market nails</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182uqbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>182pmdp</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>November nails! Mildly obsessed with all of these... 😅</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182pmdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>182ozgf</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>How can I keep this nail from splitting over and over again?</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/182ozgf/how_can_i_keep_this_nail_from_splitting_over_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>183b2kt</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Are these almost too real looking 😂</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4xjra0n4f2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>183asnx</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Frenemies forever!</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183asnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>183aqh8</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Aura nails with sparkle stickers💖</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7luwue491f2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>18330lq</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Ho ho ho 😍🎄</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3wkxmcz8d2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1832id9</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>My nails this week. As a nail tech. Winter Cat eye chrome and Thanksgiving!</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1832id9</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1832gul</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>My nails last week as a nail tech. Jade and fall iridescent chrome.</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1832gul</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1832cxx</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Simple vacay nails</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/io844zeu3d2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1832c39</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Fall nails</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8api4hn3d2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1830ots</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Obsessed with how much these press-ons matched my purse</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0awj2q2lqc2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>182zgzk</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>These remind me of the different holiday doors in the nightmare before christmas 🎃❄️🎄☠️</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5i6427tgc2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>182ydw7</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Christmas Freestyles ✨</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182ydw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>182u9fx</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>What do you think of Korean style nail stickers?? One day I’m minimalist the next day I want these 🥹</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7m6z37jzab2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>182tnbb</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Nails I created for Christmas, which one is your favourite?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182tnbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>182nq30</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Aspiring NailTech</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/182nq30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Nov 26 08:07:13 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_11_26.xlsx
+++ b/data/2023_11_26.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C943"/>
+  <dimension ref="A1:C1083"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16464,6 +16464,2386 @@
         </is>
       </c>
     </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1845joz</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Picked up this Morgan Taylor polish at Sally’s on Black Friday for $5 .</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1845joz</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1845h71</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Need some suggestions for shaping</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1845h71</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1844ri9</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>I’ve been growing them since May. So sad</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1844ri9</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>18445nh</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>help with nails curving(?)</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oiylh5a9vm2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>184039g</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>How do I stop peeling nails? Please</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/184039g</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>183y8d1</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Nail glue sticker recommendations</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183y8d1/nail_glue_sticker_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>183wsqu</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>How do you nail techs glue on charms &amp; stones without a big glue blob underneath/surrounding the charm/stone?</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183wsqu/how_do_you_nail_techs_glue_on_charms_stones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1842ies</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>first time doing red!🌹</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1842ies</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1842dty</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Got a thing for cherries</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjhxo7ddcm2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>18429o3</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>First Gel Set!</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ugrva1h7bm2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1841vnj</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1841vnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1841pjg</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Sets done by me! Very proud 🥰</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1841pjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1841l7l</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Is it safe to use jewelry glue on broken white part of nail?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1841l7l/is_it_safe_to_use_jewelry_glue_on_broken_white/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1841a5p</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Hand painted ❄️</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xmxvphg1m2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>184177h</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Mooncat - Sabertooth brushed with Orly - Sauté</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/184177h</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>18412r4</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>How can I better protect my nails</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18412r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>18412ld</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Ripple Reflect - 765 - Essie</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18412ld</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1840ic6</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>yayyy or nahhh</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dpr6ej56ul2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1840gtr</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>grippas - opinions? 🙃</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmlip39stl2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1840bb2</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Selling my Medelones gel?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1840bb2/selling_my_medelones_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>18403hb</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Velvet nails, 2nd attempt</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k600qvlfql2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>184021p</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These were SO fun to do!!!! It’s acrylic overlay on matte. </t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o60yt172ql2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>183zn9h</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>solar vs acrylic and question about nail thickness</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183zn9h/solar_vs_acrylic_and_question_about_nail_thickness/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>183zjfr</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Grey</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183zjfr</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>183z2ow</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Black nails</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183z2ow</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>183yxol</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Pretty good for an apprentice 🤩</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183yxol</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>183yxno</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Did I select the wrong shade of red?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9oeuo4xfl2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>183yw4b</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Back to my almond shape 💅🏼</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28fuv0kjfl2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>183ypoo</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>This is the best set I've done for myself so far</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xkmfkenzdl2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>183xxro</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>poly gel french shorties 🦢</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5vwdbcw67l2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>183x7vq</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>first christmas set of the year! handpainted by me</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0qcpc621l2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>183x4u0</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>New set ft. a lil bunny 🐰</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fob2jka0l2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>183wqzf</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Beautiful grey</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6nl60puwk2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>183vx94</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>new nails!!!</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/it0c5zk1qk2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>183viel</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Help: Nail polish name master list needed</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183viel/help_nail_polish_name_master_list_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>183vh99</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Loving my new set! Winter wonderland nails</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183vh99</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>183usiv</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>DIY. It’s only ok, but my GF will love it :)</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183usiv</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>183urbl</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Press on recs?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eals8lqpgk2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>183uqdj</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>christmas press ons❤️it’s my first time trying to do a peppermint swirl</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/incv5joigk2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>183u9in</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Sparkles</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl96v26rck2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>183u33a</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Wanda and Cosmo 🩷💚</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/leb5kejbbk2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>183tykg</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Stuck home with COVID - how can I fix this for now??</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfsl2js9ak2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>183tlrx</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Some recent press on sets I’ve made 😊</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183tlrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>183tlis</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Holiday Nails - Could be sooo much better!!</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183tlis</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>183tbil</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>I did these nails exactly 3 years ago but I still think they’re so cute 🦋</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183tbil</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>183t5fb</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>My Christmas nails ❤</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183t5fb</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>183sj73</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Just discovered my keyboard matches the nails</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183sj73</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>183s2p5</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>🤍🖤</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183s2p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>183rvfv</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Any recommendations on some good liner brushes?</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183rvfv/any_recommendations_on_some_good_liner_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>183ru6a</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Was feeling creative with my French chrome!</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1xu78ixsj2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>183r0on</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Glazed ombré 🍇</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mjf5wyi9mj2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>183qo5h</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>🎄💖</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmnsp4kgjj2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>183qm5q</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>A lil twist on a classic French mani</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uek7osi1jj2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>183pspn</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Glossify with cat tax</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00ky6yrecj2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>183ps52</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Did my mom’s nails for the first time (also my first time doing anyone else’s nails :p)</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t557o6pacj2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>183oyec</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Winter nails</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7gmgcik5j2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>183ou0f</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>New manicure - wave gel polishes wv107 &amp; wv117</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pzq7qpk4j2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>183opy4</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Chrome! 😍</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx54718p3j2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>183oi98</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Christmas nails😍💅🏼 one out of 3 😏</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltf02ody1j2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>183oean</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>A Purple Good Time</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlwz5upz0j2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>183o8eu</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Yay but mah 😭 hope you all like!! 🩷</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/de5v0grszi2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>183o4ss</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>I forgot to top coat one of my nails apparently and I've only noticed on my way to the airport 🙄</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/indd7z22zi2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>183nx6o</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Would be happy about opinions or suggestions</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dj2hwc2fxi2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>183lx20</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>New to press ons: can someone explain how you figure out which nail goes w/which finger?</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183lx20/new_to_press_ons_can_someone_explain_how_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>183n4i2</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Baby pink</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khghwl3tqi2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>183btrf</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Gel X help!!! Popping off day after</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183btrf/gel_x_help_popping_off_day_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1835pta</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Togepi (Pokémon) inspired nails I got today!</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1835pta</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>183mrpp</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Winter ready?</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183mrpp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>183mr1l</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>What am I doing wrong with my solid gel glue?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183mr1l/what_am_i_doing_wrong_with_my_solid_gel_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>183meqb</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Blue and Red</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183meqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>183m345</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Dreaming of a Pink Christmas</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183m345</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>183m06v</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Had to cut due to a break, so here's some short nails I did 🥲</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183m06v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>183kvm3</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>My first press ons! I love the peaches 🍑</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183kvm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>183k6qw</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Polish v Shellac</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183k6qw/polish_v_shellac/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>183ibsm</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Fav and least fav unique nail shapes</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183ibsm/fav_and_least_fav_unique_nail_shapes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>183guhw</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>My 5th attempt of doing gel nails by myself.</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouumg9nuzg2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>183gklw</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Went to a new nail tech and got Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/du48z4tewg2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>183g5w7</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Should I request that my nails be redone?</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/183g5w7/should_i_request_that_my_nails_be_redone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1845cjv</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Soft glam (and getting roasted by grandpa)</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1845cjv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>184459h</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Looking for a jelly white holo nail polish. Like this but in white?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3082acv4vm2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1843hjx</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>got my bottle of "starry-eyed" today</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1843hjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>18431om</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>“My nails are so short and nubby!!!!” The nails:</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tt9zfftcjm2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1841wpc</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Gone from embarrassed nailbiter to obsessed with my nails thanks to this sub 😭</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1841wpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1842l37</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Large Magnet Experiment for Velvet Nails</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1842l37</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>183thut</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Mooncat polish has quickly become my favorite nail polish brand! 😻</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183thut</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>18413ez</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Mooncat - Sabertooth brushed with Orly - Sauté</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18413ez</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>18411m3</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Essie LED Lamp?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18411m3/essie_led_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1840rri</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Heavenmetal by Mooncat</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uri0s8vqwl2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>183zuf3</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Starrily Mars</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p11lxb75ol2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>183yvb3</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Access Denied with a side of velociraptor</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183yvb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>183wkjq</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Dupe? Nicole OPI the next Ceo</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183wkjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>183w5m6</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>My palate cleanser didn’t even make it 24 hours</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183w5m6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>183vxzl</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>How can I make a manicure last a week or longer?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/183vxzl/how_can_i_make_a_manicure_last_a_week_or_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>183viv4</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>How long after painting my nails should I wait for nail oil?</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/183viv4/how_long_after_painting_my_nails_should_i_wait/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>183vi5f</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Lumen Wild Wings</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183vi5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>183vcx9</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>my first christmas set this year! handpainted by me! (__kmnails)</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7v7h2k1jlk2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>183vb09</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>November Mooncat mani dump (short nails)</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183vb09</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>183v34n</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Blinding holo by a-England *PR*</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1exm087jk2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>183uc5e</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Morocco ! 💓💓</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183uc5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>183tvv5</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Tips for using chunky glitter toppers?</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkzwzmtn9k2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>183t1mx</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Ethereal ✨</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u7xx4f3u2k2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>183t1ip</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Wish upon a star</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183t1ip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>183sv7v</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Mama</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183sv7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>183rz77</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>[Gifted] Holo Taco: Midnight Owl 🌙🔮</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183rz77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>183rylc</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>all the gold sparkle I could muster 🌟</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/82wpfv3ytj2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>183rx05</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Thanksgiving Paddle Trip - Later Alligator</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2hu5q1ktj2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>183rp0n</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>French Manicure</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183rp0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>183rloz</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Maniology topcoat shrinkage</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183rloz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>183rjyn</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Best NON quick-dry top coat?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/183rjyn/best_non_quickdry_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>183rd68</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>ILNP shooting stars 💫</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183rd68</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>183r9vq</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Can’t believe I almost didn’t get this</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/91oqihqaoj2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>183r63c</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>{PR} Skiing is Believing by KB Shimmer 😍</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2r8zdbhnj2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>183r31i</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Opal Sunset</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183r31i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>183qvqc</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Goodbye Autumn 🍂</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183qvqc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>183qtcm</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>First time using mooncat polish</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183qtcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>183qq2p</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Mooncat Sabertooth ✨</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183qq2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>183qorg</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Mom's Thanksgiving Mani 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkz5250mjj2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>183qgcx</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Don't you love when your manicure inspires the whole outfit?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/GS9GqBk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>183q4v8</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Mooncat Antivenom, 1 week old!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183q4v8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>183pw73</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Zoya Tabitha - no base coat, Seche Vite quick dry topcoat. Beautiful and dark Christmas green</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fkioe9zcj2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>183pe5x</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Bitten with Lovebird topper by ILNP</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/le3m9yy39j2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>183oqhe</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>🩷💕💞💓💗 Mooncat has amazed me once again 🩷💕💞💓💗</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r53vaext3j2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>183nvyb</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>This is the multi-est multichrome</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183nvyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>18381si</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>My green nails done in August.</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18381si</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>183mm2j</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Faceted bottle NHC polish 🤩</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/tV6MVYq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>183mce8</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Beware the Kraken!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ewzwu0ahki2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>183l1uj</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Picked up this polish just to try the U magnet hack</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rs80vgo39i2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>183k4mx</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Sally Hansen Night Lily Dupe</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3036opq0i2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>183k4mh</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Glowy neutral</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183k4mh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>183gwlr</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Nails break even through gel polish, any advice?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrgja0rk0h2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>183g5ks</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Ilnp reward points</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/183g5ks/ilnp_reward_points/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>183fvmt</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Birthday Skittle!</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oq9tv3xkng2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>183f4uw</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Does anyone know where I can find a polish similar to Lacquer Lust's Unicorn Porn?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/183f4uw/does_anyone_know_where_i_can_find_a_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1845eoh</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Are you guys into Coquette nails?</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdwtms7u9n2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>183ygjf</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>A little something extra 🎁</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183ygjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>183vf0t</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Merry Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y23os7bzlk2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>183tes2</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Advice?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/183tes2/advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>183rmsv</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Mystery Nail Art Challenge Part 15</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://youtu.be/QCSDJ3SgR-Q?si=uFiLIXHixzEw_Lfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>183r55y</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Reindeer nails for the winter!</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183r55y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>183pcl1</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Simple summer nail designs by me! ✌🏼</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/183pcl1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>